<commit_message>
added uml diagram and updated gitignore to ignore intermediate excel files
</commit_message>
<xml_diff>
--- a/dataSet.xlsx
+++ b/dataSet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\ISU\Honors\HonorsProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\ISU\Honors\HonorsProject\ComedyCollegeAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD26F7EB-1699-4AA1-839E-04E63BD444A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA58D17F-807E-4341-AFEF-90FB766A8B2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{9DCEE0AE-6EE9-4686-BBF9-5BADB3A4DC01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9DCEE0AE-6EE9-4686-BBF9-5BADB3A4DC01}"/>
   </bookViews>
   <sheets>
     <sheet name="Comedian" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD73E9F6-7E7E-4006-A81E-40B4F6B838A3}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -524,30 +524,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3C8D3A-EB73-4B65-8AAF-C3DAD677A218}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -632,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB48393A-C823-4075-B153-1700C22DDE52}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>